<commit_message>
Changes in reader, voter and reader test
changes in the iterface, and error correction
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x15 xr">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cursos\asw\1516\censusesI2\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9" documentId="06430DCD22CD0E9B3883142183B54C466B6F2389"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8370" windowHeight="2370"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162912"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -113,7 +114,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -391,14 +392,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x14ac xr xr2" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
@@ -406,7 +407,7 @@
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -420,7 +421,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -434,7 +435,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -448,7 +449,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -464,9 +465,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>

</xml_diff>

<commit_message>
Modify Gateway to return a list of non repeated voters  only.
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x15 xr">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cursos\asw\1516\censusesI2\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dax\IdeaProjects\censusesI2\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="06430DCD22CD0E9B3883142183B54C466B6F2389"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8370" windowHeight="2370"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162912"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>NIF</t>
   </si>
@@ -64,12 +63,27 @@
   </si>
   <si>
     <t>anatorres@hotmail.com</t>
+  </si>
+  <si>
+    <t>sadsad@sda.com</t>
+  </si>
+  <si>
+    <t>Donald Trump</t>
+  </si>
+  <si>
+    <t>00000000X</t>
+  </si>
+  <si>
+    <t>Usain bolt</t>
+  </si>
+  <si>
+    <t>asddN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -392,14 +406,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x14ac xr xr2" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
@@ -407,7 +421,7 @@
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -421,7 +435,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -435,7 +449,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -449,7 +463,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -461,15 +475,45 @@
       </c>
       <c r="D4">
         <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>